<commit_message>
Implement add new stock with PDF
</commit_message>
<xml_diff>
--- a/Files/Stocks/xlsx Files/EREGL.IS.xlsx
+++ b/Files/Stocks/xlsx Files/EREGL.IS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -34,7 +34,16 @@
     <t>Total</t>
   </si>
   <si>
-    <t>2023-07-28</t>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>26-10-2022</t>
+  </si>
+  <si>
+    <t>27-10-2022</t>
+  </si>
+  <si>
+    <t>08-11-2022</t>
   </si>
   <si>
     <t>-</t>
@@ -401,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,45 +435,100 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>30.28</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2">
-        <v>40</v>
+        <v>302.8</v>
+      </c>
+      <c r="G2">
+        <v>0.63</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>30.86</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>462.9</v>
+      </c>
+      <c r="G3">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>360</v>
+      </c>
+      <c r="G4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>40</v>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>32.163</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>1125.7</v>
+      </c>
+      <c r="G5">
+        <v>2.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>